<commit_message>
Actualizacion terminada segun nuestro nuevo modelo para la solucion del problema de reservas en conjuntos residenciales al dia en la seccion 8 event storming
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Modelo de dominio anémico de contextos-VictusResidencias.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Modelo de dominio anémico de contextos-VictusResidencias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\trabajoDOO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1789F93D-7989-4E21-B117-A4C3AE034A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C7ADEF-25B3-46F3-A8C5-B1005FE667E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{082AFB46-52C9-4E4C-AE4E-19443AA1B53B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{082AFB46-52C9-4E4C-AE4E-19443AA1B53B}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="3" r:id="rId1"/>
@@ -950,6 +950,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1055,6 +1061,21 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1079,22 +1100,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1107,21 +1122,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1148,22 +1148,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>210536</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>10191</xdr:rowOff>
+      <xdr:colOff>343894</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>29284</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4778A2CC-7D37-F19E-94A2-B72B66404A32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA9D2E82-FF5A-357B-B457-4B26C11893C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1172,65 +1172,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="190500"/>
-          <a:ext cx="7068536" cy="4772691"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>210536</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>48350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BEF9D12-7A66-D739-A433-A4114727C5D6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="190500"/>
-          <a:ext cx="7068536" cy="5191850"/>
+          <a:off x="76200" y="95250"/>
+          <a:ext cx="7125694" cy="5077534"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1593,20 +1543,20 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="79.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="48"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="50"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
@@ -1614,7 +1564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1622,7 +1572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -1630,13 +1580,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>16</v>
       </c>
@@ -1644,7 +1594,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>17</v>
       </c>
@@ -1652,7 +1602,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>18</v>
       </c>
@@ -1660,7 +1610,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +1618,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>20</v>
       </c>
@@ -1676,7 +1626,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>21</v>
       </c>
@@ -1684,7 +1634,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>22</v>
       </c>
@@ -1708,109 +1658,109 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="13" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="58" style="30" customWidth="1"/>
-    <col min="19" max="19" width="17.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="13"/>
+    <col min="19" max="19" width="17.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="96">
+      <c r="B1" s="101">
         <f>'[1]Configuración Apuestas'!D10</f>
         <v>0</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="97"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="101"/>
+      <c r="R1" s="101"/>
+      <c r="S1" s="102"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="79"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="81"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="86" t="s">
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="88" t="s">
+      <c r="S3" s="95" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
@@ -1862,10 +1812,10 @@
       <c r="Q4" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="98"/>
-      <c r="S4" s="99"/>
-    </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R4" s="103"/>
+      <c r="S4" s="104"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26"/>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
@@ -1904,10 +1854,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1922,43 +1872,43 @@
       <selection activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="2"/>
+    <col min="1" max="1" width="36.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="59"/>
-    </row>
-    <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="60"/>
+      <c r="D1" s="61"/>
+    </row>
+    <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="62"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
+      <c r="C2" s="63"/>
+      <c r="D2" s="64"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1972,127 +1922,127 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="71" t="s">
         <v>66</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="72" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="68"/>
-      <c r="B6" s="69"/>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="70"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="70"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="68"/>
-      <c r="B7" s="69"/>
+      <c r="D6" s="72"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="70"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="70"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="68"/>
-      <c r="B8" s="69"/>
+      <c r="D7" s="72"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="70"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="70"/>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
-      <c r="B9" s="69"/>
+      <c r="D8" s="72"/>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="70"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="70"/>
-    </row>
-    <row r="10" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="68"/>
-      <c r="B10" s="69"/>
+      <c r="D9" s="72"/>
+    </row>
+    <row r="10" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="70"/>
-    </row>
-    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="66" t="s">
+      <c r="D10" s="72"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="69" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="68" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="66"/>
-      <c r="B12" s="67"/>
+    <row r="12" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="68"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="66"/>
-    </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="66"/>
-      <c r="B13" s="67"/>
+      <c r="D12" s="68"/>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="68"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="66"/>
-    </row>
-    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="49" t="s">
+      <c r="D13" s="68"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="54" t="s">
         <v>65</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="57" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="53"/>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="52"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="56"/>
-    </row>
-    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
-      <c r="B16" s="53"/>
+      <c r="D15" s="58"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="52"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="56"/>
-    </row>
-    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
-      <c r="B17" s="54"/>
+      <c r="D16" s="58"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="53"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="57"/>
+      <c r="D17" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2148,112 +2098,112 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="38.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="13"/>
+    <col min="7" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="71" t="str">
+      <c r="B1" s="73" t="str">
         <f>Contextos!B5</f>
         <v xml:space="preserve"> Gestión de Conjuntos residenciales</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="72"/>
-    </row>
-    <row r="2" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="74"/>
+    </row>
+    <row r="2" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="75" t="str">
         <f>Contextos!D5</f>
         <v>Contexto cuya motivación es Gestionar la estructura física y los recursos disponibles en cada conjunto residencial. Aquí se manejan los datos sobre qué conjuntos existen, dónde están ubicados, qué recursos ofrecen según una Agenda con respectivos turnos para cada zona.</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="74"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="75" t="str">
+      <c r="B3" s="77" t="str">
         <f>Contextos!A5</f>
         <v>Core/Básico</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="81"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="81" t="s">
+      <c r="E5" s="82"/>
+      <c r="F5" s="83" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="81"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="83"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="80"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="81"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F7" s="83"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>41</v>
       </c>
@@ -2275,7 +2225,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>23</v>
       </c>
@@ -2297,7 +2247,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>68</v>
       </c>
@@ -2319,7 +2269,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>41</v>
       </c>
@@ -2341,7 +2291,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>70</v>
       </c>
@@ -2363,7 +2313,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>23</v>
       </c>
@@ -2415,117 +2365,117 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D386A343-6D12-4FEA-AEEF-63E15D63FE79}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="13"/>
+    <col min="7" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="71" t="str">
+      <c r="B1" s="73" t="str">
         <f>Contextos!B11</f>
         <v>Gestión de Residentes</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="72"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="74"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="75" t="str">
         <f>Contextos!D11</f>
         <v>Contexto cuya motivación es encargarce de manejar la información de los residentes, incluidas sus identificaciones, contacto, y la relación entre el residente y su residencia dentro del conjunto.</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="74"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="75" t="str">
+      <c r="B3" s="77" t="str">
         <f>Contextos!A11</f>
         <v>Core/Básico</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="81"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="81" t="s">
+      <c r="E5" s="82"/>
+      <c r="F5" s="83" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="81"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="83"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="80"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="81"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F7" s="83"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>63</v>
       </c>
@@ -2547,7 +2497,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>25</v>
       </c>
@@ -2603,113 +2553,113 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="13"/>
+    <col min="7" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="71" t="str">
+      <c r="B1" s="73" t="str">
         <f>Contextos!B14</f>
         <v>Reservas</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="72"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="74"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="75" t="str">
         <f>Contextos!D14</f>
         <v>Contexto cuya intención enfocarse en la gestión del proceso de reservas de los recursos, incluyendo la disponibilidad de los recursos y las reservas que los residentes realizan.</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="74"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="75" t="str">
+      <c r="B3" s="77" t="str">
         <f>Contextos!A14</f>
         <v>Core/Básico</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="81"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="81" t="s">
+      <c r="E5" s="82"/>
+      <c r="F5" s="83" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="81"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="83"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="80"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="81"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F7" s="83"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>42</v>
       </c>
@@ -2731,7 +2681,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>69</v>
       </c>
@@ -2753,7 +2703,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>25</v>
       </c>
@@ -2809,107 +2759,107 @@
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="13" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="58" style="30" customWidth="1"/>
-    <col min="19" max="19" width="17.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="13"/>
+    <col min="19" max="19" width="17.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="82" t="str">
+      <c r="B1" s="89" t="str">
         <f>Reservas!D8</f>
         <v>Reserva-0001</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="83"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="79"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="90"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="81"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="86" t="s">
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="88" t="s">
+      <c r="S3" s="95" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>29</v>
       </c>
@@ -2961,14 +2911,14 @@
       <c r="Q4" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="87"/>
-      <c r="S4" s="89"/>
-    </row>
-    <row r="5" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="90" t="s">
+      <c r="R4" s="94"/>
+      <c r="S4" s="96"/>
+    </row>
+    <row r="5" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="85" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="36" t="s">
@@ -3009,14 +2959,14 @@
         <f>_xlfn.CONCAT("Atributo que contiene la informacion del identificador de un ",B5,"  en el contexto de ",A5,".")</f>
         <v>Atributo que contiene la informacion del identificador de un ConjuntoResidencial  en el contexto de Gestión de Conjuntos residenciales.</v>
       </c>
-      <c r="S5" s="93" t="str">
+      <c r="S5" s="87" t="str">
         <f>B7</f>
         <v>ZonaComun</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="90"/>
-      <c r="B6" s="91"/>
+    <row r="6" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="36" t="s">
         <v>59</v>
       </c>
@@ -3055,11 +3005,11 @@
         <f>_xlfn.CONCAT("Atributo que contiene la información del nombre de un ",B5," en el contexto de ",A5," asociado al residente con el identificador' ",J6,"'.")</f>
         <v>Atributo que contiene la información del nombre de un ConjuntoResidencial en el contexto de Gestión de Conjuntos residenciales asociado al residente con el identificador' nombreConjuntoResidencial'.</v>
       </c>
-      <c r="S6" s="94"/>
-    </row>
-    <row r="7" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="90"/>
-      <c r="B7" s="92" t="s">
+      <c r="S6" s="88"/>
+    </row>
+    <row r="7" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="84"/>
+      <c r="B7" s="86" t="s">
         <v>42</v>
       </c>
       <c r="C7" s="38" t="s">
@@ -3100,11 +3050,11 @@
         <f>_xlfn.CONCAT("Atributo que contiene la informacion del identificador de un ",B7,"  en el contexto de ",A5,".")</f>
         <v>Atributo que contiene la informacion del identificador de un ZonaComun  en el contexto de Gestión de Conjuntos residenciales.</v>
       </c>
-      <c r="S7" s="94"/>
-    </row>
-    <row r="8" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="90"/>
-      <c r="B8" s="92"/>
+      <c r="S7" s="88"/>
+    </row>
+    <row r="8" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="84"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="38" t="s">
         <v>59</v>
       </c>
@@ -3143,11 +3093,11 @@
         <f>_xlfn.CONCAT("Atributo que contiene la información del nombre de un ",B7," en el contexto de ",A5," asociado a la reserva con el identificador' ",J8,"'.")</f>
         <v>Atributo que contiene la información del nombre de un ZonaComun en el contexto de Gestión de Conjuntos residenciales asociado a la reserva con el identificador' nombreZonaComun'.</v>
       </c>
-      <c r="S8" s="94"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="90"/>
-      <c r="B9" s="92"/>
+      <c r="S8" s="88"/>
+    </row>
+    <row r="9" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="84"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="38" t="s">
         <v>64</v>
       </c>
@@ -3168,9 +3118,9 @@
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
       <c r="R9" s="39"/>
-      <c r="S9" s="94"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="S9" s="88"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A5:A9"/>
@@ -3196,107 +3146,107 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="21" style="13" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="13" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="58" style="30" customWidth="1"/>
-    <col min="19" max="19" width="17.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="13"/>
+    <col min="19" max="19" width="17.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="82" t="str">
+      <c r="B1" s="89" t="str">
         <f>Reservas!D9</f>
         <v>Reserva-0002</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="83"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="79"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="90"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="81"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="86" t="s">
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="88" t="s">
+      <c r="S3" s="95" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>29</v>
       </c>
@@ -3348,14 +3298,14 @@
       <c r="Q4" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="87"/>
-      <c r="S4" s="89"/>
-    </row>
-    <row r="5" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="90" t="s">
+      <c r="R4" s="94"/>
+      <c r="S4" s="96"/>
+    </row>
+    <row r="5" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="97" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="36" t="s">
@@ -3392,18 +3342,18 @@
       <c r="O5" s="36"/>
       <c r="P5" s="36"/>
       <c r="Q5" s="36"/>
-      <c r="R5" s="100" t="str">
+      <c r="R5" s="47" t="str">
         <f>_xlfn.CONCAT("Atributo que contiene la informacion del identificador de un ",B5,"  en el contexto de ",A5,".")</f>
         <v>Atributo que contiene la informacion del identificador de un Agenda  en el contexto de Conjuntos Residenciales.</v>
       </c>
-      <c r="S5" s="102" t="str">
+      <c r="S5" s="98" t="str">
         <f>B7</f>
         <v>Turno</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="90"/>
-      <c r="B6" s="95"/>
+    <row r="6" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="84"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="36" t="s">
         <v>59</v>
       </c>
@@ -3438,15 +3388,15 @@
       <c r="O6" s="36"/>
       <c r="P6" s="36"/>
       <c r="Q6" s="36"/>
-      <c r="R6" s="100" t="str">
+      <c r="R6" s="47" t="str">
         <f>_xlfn.CONCAT("Atributo que contiene la información del nombre de un ",B5," en el contexto de ",A5," asociado al residente con el identificador' ",J6,"'.")</f>
         <v>Atributo que contiene la información del nombre de un Agenda en el contexto de Conjuntos Residenciales asociado al residente con el identificador' nombreAgenda'.</v>
       </c>
-      <c r="S6" s="103"/>
-    </row>
-    <row r="7" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="90"/>
-      <c r="B7" s="92" t="s">
+      <c r="S6" s="99"/>
+    </row>
+    <row r="7" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="84"/>
+      <c r="B7" s="86" t="s">
         <v>69</v>
       </c>
       <c r="C7" s="38" t="s">
@@ -3483,15 +3433,15 @@
       <c r="O7" s="38"/>
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
-      <c r="R7" s="101" t="str">
+      <c r="R7" s="48" t="str">
         <f>_xlfn.CONCAT("Atributo que contiene la informacion del identificador de un ",B7,"  en el contexto de ",A5,".")</f>
         <v>Atributo que contiene la informacion del identificador de un Turno  en el contexto de Conjuntos Residenciales.</v>
       </c>
-      <c r="S7" s="103"/>
-    </row>
-    <row r="8" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="90"/>
-      <c r="B8" s="92"/>
+      <c r="S7" s="99"/>
+    </row>
+    <row r="8" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="84"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="38" t="s">
         <v>59</v>
       </c>
@@ -3526,15 +3476,15 @@
       <c r="O8" s="38"/>
       <c r="P8" s="38"/>
       <c r="Q8" s="38"/>
-      <c r="R8" s="101" t="str">
+      <c r="R8" s="48" t="str">
         <f>_xlfn.CONCAT("Atributo que contiene la información del nombre de un ",B7," en el contexto de ",A5," asociado a la reserva con el identificador' ",J8,"'.")</f>
         <v>Atributo que contiene la información del nombre de un Turno en el contexto de Conjuntos Residenciales asociado a la reserva con el identificador' nombreTurno'.</v>
       </c>
-      <c r="S8" s="103"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="90"/>
-      <c r="B9" s="92"/>
+      <c r="S8" s="99"/>
+    </row>
+    <row r="9" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="84"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="38" t="s">
         <v>93</v>
       </c>
@@ -3554,10 +3504,10 @@
       <c r="O9" s="38"/>
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
-      <c r="R9" s="101"/>
-      <c r="S9" s="104"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="100"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A5:A9"/>
@@ -3579,111 +3529,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E4C5E7-072D-46C9-A943-F12FD1E94927}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="21" style="13" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="13" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="58" style="30" customWidth="1"/>
-    <col min="19" max="19" width="17.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="13"/>
+    <col min="19" max="19" width="17.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="82" t="str">
+      <c r="B1" s="89" t="str">
         <f>Reservas!D9</f>
         <v>Reserva-0002</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="83"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="79"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="90"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="81"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="86" t="s">
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="88" t="s">
+      <c r="S3" s="95" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>29</v>
       </c>
@@ -3735,14 +3685,14 @@
       <c r="Q4" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="87"/>
-      <c r="S4" s="89"/>
-    </row>
-    <row r="5" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="90" t="s">
+      <c r="R4" s="94"/>
+      <c r="S4" s="96"/>
+    </row>
+    <row r="5" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="97" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="36" t="s">
@@ -3779,18 +3729,18 @@
       <c r="O5" s="36"/>
       <c r="P5" s="36"/>
       <c r="Q5" s="36"/>
-      <c r="R5" s="100" t="str">
+      <c r="R5" s="47" t="str">
         <f>_xlfn.CONCAT("Atributo que contiene la informacion del identificador de un ",B5,"  en el contexto de ",A5,".")</f>
         <v>Atributo que contiene la informacion del identificador de un ConjuntoResidencial  en el contexto de Gestión de Residentes.</v>
       </c>
-      <c r="S5" s="102" t="str">
+      <c r="S5" s="98" t="str">
         <f>B7</f>
         <v>Residente</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="90"/>
-      <c r="B6" s="95"/>
+    <row r="6" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="84"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="36" t="s">
         <v>59</v>
       </c>
@@ -3825,15 +3775,15 @@
       <c r="O6" s="36"/>
       <c r="P6" s="36"/>
       <c r="Q6" s="36"/>
-      <c r="R6" s="100" t="str">
+      <c r="R6" s="47" t="str">
         <f>_xlfn.CONCAT("Atributo que contiene la información del nombre de un ",B5," en el contexto de ",A5," asociado al residente con el identificador' ",J6,"'.")</f>
         <v>Atributo que contiene la información del nombre de un ConjuntoResidencial en el contexto de Gestión de Residentes asociado al residente con el identificador' nombreConjuntoResidencial'.</v>
       </c>
-      <c r="S6" s="103"/>
-    </row>
-    <row r="7" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="90"/>
-      <c r="B7" s="92" t="s">
+      <c r="S6" s="99"/>
+    </row>
+    <row r="7" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="84"/>
+      <c r="B7" s="86" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="38" t="s">
@@ -3870,15 +3820,15 @@
       <c r="O7" s="38"/>
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
-      <c r="R7" s="101" t="str">
+      <c r="R7" s="48" t="str">
         <f>_xlfn.CONCAT("Atributo que contiene la informacion del identificador de un ",B7,"  en el contexto de ",A5,".")</f>
         <v>Atributo que contiene la informacion del identificador de un Residente  en el contexto de Gestión de Residentes.</v>
       </c>
-      <c r="S7" s="103"/>
-    </row>
-    <row r="8" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="90"/>
-      <c r="B8" s="92"/>
+      <c r="S7" s="99"/>
+    </row>
+    <row r="8" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="84"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="38" t="s">
         <v>59</v>
       </c>
@@ -3913,15 +3863,15 @@
       <c r="O8" s="38"/>
       <c r="P8" s="38"/>
       <c r="Q8" s="38"/>
-      <c r="R8" s="101" t="str">
+      <c r="R8" s="48" t="str">
         <f>_xlfn.CONCAT("Atributo que contiene la información del nombre de un ",B7," en el contexto de ",A5," asociado a la reserva con el identificador' ",J8,"'.")</f>
         <v>Atributo que contiene la información del nombre de un Residente en el contexto de Gestión de Residentes asociado a la reserva con el identificador' nombreResidente'.</v>
       </c>
-      <c r="S8" s="103"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="90"/>
-      <c r="B9" s="92"/>
+      <c r="S8" s="99"/>
+    </row>
+    <row r="9" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="84"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="38" t="s">
         <v>93</v>
       </c>
@@ -3941,22 +3891,22 @@
       <c r="O9" s="38"/>
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
-      <c r="R9" s="101"/>
-      <c r="S9" s="104"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="100"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="S5:S9"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="B1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="J3:Q3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="S5:S9"/>
-    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>